<commit_message>
update tally for printing
</commit_message>
<xml_diff>
--- a/tests/dydParse/caseTally.xlsx
+++ b/tests/dydParse/caseTally.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heyth\source\repos\thadhaines\PSLTDSim\tests\dydParse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jhaines\source\Repos\thadhaines\PSLTDSim\tests\dydParse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="raw highlight" sheetId="1" r:id="rId1"/>
     <sheet name="zeros removed" sheetId="2" r:id="rId2"/>
+    <sheet name="for printing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="195">
   <si>
     <t>Finished Processing 180033 Lines.</t>
   </si>
@@ -598,12 +599,24 @@
   </si>
   <si>
     <t>2018 heavy spring</t>
+  </si>
+  <si>
+    <t>Finished Processing 180,033 Lines.</t>
+  </si>
+  <si>
+    <t>Finished Processing 180,018 Lines.</t>
+  </si>
+  <si>
+    <t>Finished Processing 177,894 Lines.</t>
+  </si>
+  <si>
+    <t>Finished Processing 153,160 Lines.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -924,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F45" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3025,6 +3038,852 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D63"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" t="s">
+        <v>130</v>
+      </c>
+      <c r="D53" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
+      <c r="D55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" t="s">
+        <v>133</v>
+      </c>
+      <c r="D56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" t="s">
+        <v>135</v>
+      </c>
+      <c r="D58" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" t="s">
+        <v>137</v>
+      </c>
+      <c r="D60" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" t="s">
+        <v>138</v>
+      </c>
+      <c r="D61" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>